<commit_message>
levee report bug fix again
</commit_message>
<xml_diff>
--- a/Lamia/DBASE/create/Base2_0_6.xlsx
+++ b/Lamia/DBASE/create/Base2_0_6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patrice.verchere\PycharmProjects\Lamia\Lamia\DBASE\create\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patrice.verchere\OneDrive - ARTELIA\PycharmProjects\Lamia\Lamia\DBASE\create\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFCB7C3-DCDC-4798-B265-FF1ED640E230}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7DFCB7C3-DCDC-4798-B265-FF1ED640E230}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D8B7327B-4353-4BA3-AC4F-5A77D8355B6F}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="767" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="767" firstSheet="8" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="18" r:id="rId1"/>
@@ -63,7 +63,7 @@
     <sheet name="10_siartelia" sheetId="49" r:id="rId48"/>
     <sheet name="11_utilisateur" sheetId="50" r:id="rId49"/>
   </sheets>
-  <calcPr calcId="0" iterateCount="1"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -1876,13 +1876,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1969,35 +1976,36 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" quotePrefix="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" quotePrefix="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
@@ -4242,8 +4250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4495,7 +4503,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="19" t="s">
         <v>280</v>
       </c>
       <c r="B27" t="s">
@@ -9001,7 +9009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding the voice recorder pluging
</commit_message>
<xml_diff>
--- a/Lamia/DBASE/create/Base2_0_6.xlsx
+++ b/Lamia/DBASE/create/Base2_0_6.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patrice.verchere\PycharmProjects\Lamia\Lamia\DBASE\create\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raphael.beck-protoy\Documents\Git\Lamia\Lamia\DBASE\create\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFCB7C3-DCDC-4798-B265-FF1ED640E230}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="767" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="767" firstSheet="18" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="18" r:id="rId1"/>
@@ -34,36 +33,37 @@
     <sheet name="04_Profil" sheetId="20" r:id="rId19"/>
     <sheet name="05_Graphique" sheetId="21" r:id="rId20"/>
     <sheet name="05_Modele" sheetId="22" r:id="rId21"/>
-    <sheet name="05_Photo" sheetId="23" r:id="rId22"/>
-    <sheet name="05_Rapport" sheetId="24" r:id="rId23"/>
-    <sheet name="05_Rasters" sheetId="25" r:id="rId24"/>
-    <sheet name="05_Topographie" sheetId="26" r:id="rId25"/>
-    <sheet name="05_Travaux" sheetId="27" r:id="rId26"/>
-    <sheet name="06_Graphiquedata" sheetId="28" r:id="rId27"/>
-    <sheet name="06_Pointtopo" sheetId="29" r:id="rId28"/>
-    <sheet name="06_Tcetudetravaux" sheetId="30" r:id="rId29"/>
-    <sheet name="06_Tcobjetintervenant" sheetId="31" r:id="rId30"/>
-    <sheet name="06_Tcobjetressource" sheetId="32" r:id="rId31"/>
-    <sheet name="06_Tcobjetzonegeo" sheetId="33" r:id="rId32"/>
-    <sheet name="06_Tctravauxdescriptionsystem" sheetId="34" r:id="rId33"/>
-    <sheet name="10_auth_group" sheetId="35" r:id="rId34"/>
-    <sheet name="10_auth_group_permissions" sheetId="36" r:id="rId35"/>
-    <sheet name="10_auth_permission" sheetId="37" r:id="rId36"/>
-    <sheet name="10_auth_user" sheetId="38" r:id="rId37"/>
-    <sheet name="10_auth_user_groups" sheetId="39" r:id="rId38"/>
-    <sheet name="10_auth_user_user_permissions" sheetId="40" r:id="rId39"/>
-    <sheet name="10_bdd" sheetId="41" r:id="rId40"/>
-    <sheet name="10_carto_layer" sheetId="42" r:id="rId41"/>
-    <sheet name="10_django_admin_log" sheetId="43" r:id="rId42"/>
-    <sheet name="10_django_content_type" sheetId="44" r:id="rId43"/>
-    <sheet name="10_django_migrations" sheetId="45" r:id="rId44"/>
-    <sheet name="10_django_session" sheetId="46" r:id="rId45"/>
-    <sheet name="10_messagetiers" sheetId="47" r:id="rId46"/>
-    <sheet name="10_projet" sheetId="48" r:id="rId47"/>
-    <sheet name="10_siartelia" sheetId="49" r:id="rId48"/>
-    <sheet name="11_utilisateur" sheetId="50" r:id="rId49"/>
+    <sheet name="05_Audio" sheetId="51" r:id="rId22"/>
+    <sheet name="05_Photo" sheetId="23" r:id="rId23"/>
+    <sheet name="05_Rapport" sheetId="24" r:id="rId24"/>
+    <sheet name="05_Rasters" sheetId="25" r:id="rId25"/>
+    <sheet name="05_Topographie" sheetId="26" r:id="rId26"/>
+    <sheet name="05_Travaux" sheetId="27" r:id="rId27"/>
+    <sheet name="06_Graphiquedata" sheetId="28" r:id="rId28"/>
+    <sheet name="06_Pointtopo" sheetId="29" r:id="rId29"/>
+    <sheet name="06_Tcetudetravaux" sheetId="30" r:id="rId30"/>
+    <sheet name="06_Tcobjetintervenant" sheetId="31" r:id="rId31"/>
+    <sheet name="06_Tcobjetressource" sheetId="32" r:id="rId32"/>
+    <sheet name="06_Tcobjetzonegeo" sheetId="33" r:id="rId33"/>
+    <sheet name="06_Tctravauxdescriptionsystem" sheetId="34" r:id="rId34"/>
+    <sheet name="10_auth_group" sheetId="35" r:id="rId35"/>
+    <sheet name="10_auth_group_permissions" sheetId="36" r:id="rId36"/>
+    <sheet name="10_auth_permission" sheetId="37" r:id="rId37"/>
+    <sheet name="10_auth_user" sheetId="38" r:id="rId38"/>
+    <sheet name="10_auth_user_groups" sheetId="39" r:id="rId39"/>
+    <sheet name="10_auth_user_user_permissions" sheetId="40" r:id="rId40"/>
+    <sheet name="10_bdd" sheetId="41" r:id="rId41"/>
+    <sheet name="10_carto_layer" sheetId="42" r:id="rId42"/>
+    <sheet name="10_django_admin_log" sheetId="43" r:id="rId43"/>
+    <sheet name="10_django_content_type" sheetId="44" r:id="rId44"/>
+    <sheet name="10_django_migrations" sheetId="45" r:id="rId45"/>
+    <sheet name="10_django_session" sheetId="46" r:id="rId46"/>
+    <sheet name="10_messagetiers" sheetId="47" r:id="rId47"/>
+    <sheet name="10_projet" sheetId="48" r:id="rId48"/>
+    <sheet name="10_siartelia" sheetId="49" r:id="rId49"/>
+    <sheet name="11_utilisateur" sheetId="50" r:id="rId50"/>
   </sheets>
-  <calcPr calcId="0" iterateCount="1"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1784" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="587">
   <si>
     <t>#DJAN</t>
   </si>
@@ -1812,77 +1812,48 @@
     <t>courriel</t>
   </si>
   <si>
-    <t>float_1</t>
-  </si>
-  <si>
-    <t>float_2</t>
-  </si>
-  <si>
-    <t>float_3</t>
-  </si>
-  <si>
-    <t>float_4</t>
-  </si>
-  <si>
-    <t>float_5</t>
-  </si>
-  <si>
-    <t>float_6</t>
-  </si>
-  <si>
-    <t>float_7</t>
-  </si>
-  <si>
-    <t>float_8</t>
-  </si>
-  <si>
-    <t>float_9</t>
-  </si>
-  <si>
-    <t>float_10</t>
-  </si>
-  <si>
-    <t>string_1</t>
-  </si>
-  <si>
-    <t>string_2</t>
-  </si>
-  <si>
-    <t>string_3</t>
-  </si>
-  <si>
-    <t>string_4</t>
-  </si>
-  <si>
-    <t>string_5</t>
-  </si>
-  <si>
-    <t>string_6</t>
-  </si>
-  <si>
-    <t>string_7</t>
-  </si>
-  <si>
-    <t>string_8</t>
-  </si>
-  <si>
-    <t>string_9</t>
-  </si>
-  <si>
-    <t>string_10</t>
+    <t>pk_audio</t>
+  </si>
+  <si>
+    <t>id_audio</t>
+  </si>
+  <si>
+    <t>typeaudio</t>
+  </si>
+  <si>
+    <t>SELECT Audio.*, Ressource.*, Objet.*  FROM Audio INNER JOIN Ressource ON Audio.lpk_ressource = Ressource.pk_ressource INNER JOIN Objet ON Ressource.lpk_objet = Objet.pk_objet WHERE Objet.lpk_revision_end IS NULL  AND Objet.datetimedestruction IS NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT Audio.*, Ressource.*, Objet.*   FROM Audio INNER JOIN Ressource ON Audio.lpk_ressource = Ressource.pk_ressource INNER JOIN Objet ON Ressource.lpk_objet = Objet.pk_objet</t>
+  </si>
+  <si>
+    <t>05_Audio</t>
+  </si>
+  <si>
+    <t>id_commentaire</t>
+  </si>
+  <si>
+    <t>id_table</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1969,44 +1940,45 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" quotePrefix="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" quotePrefix="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="3"/>
+    <cellStyle name="Normal 4" xfId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2097,23 +2069,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2149,23 +2104,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2341,11 +2279,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,244 +2486,253 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>375</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>376</v>
+        <v>584</v>
+      </c>
+      <c r="B25" s="5" t="str">
+        <f>HYPERLINK('05_Audio'!A1)</f>
+        <v>#DJAN</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>415</v>
+        <v>392</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>416</v>
+        <v>393</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>440</v>
+        <v>416</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>496</v>
+        <v>471</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>497</v>
+        <v>472</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>543</v>
+        <v>531</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>558</v>
+        <v>543</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>559</v>
+        <v>544</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>558</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>561</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B48" s="5" t="s">
         <v>562</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" location="'00_Basedonnees'!A1" display="'00_Basedonnees'!A1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" location="'00_Revision'!A1" display="'00_Revision'!A1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B3" location="'01_Objet'!A1" display="'01_Objet'!A1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B4" location="'02_Descriptionsystem'!A1" display="'02_Descriptionsystem'!A1" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B5" location="'02_Evenement'!A1" display="'02_Evenement'!A1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B6" location="'02_Marche'!A1" display="'02_Marche'!A1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B7" location="'02_Zonegeo'!A1" display="'02_Zonegeo'!A1" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B8" location="'03_Desordre'!A1" display="'03_Desordre'!A1" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B9" location="'03_Interventiontiers'!A1" display="'03_Interventiontiers'!A1" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B10" location="'03_Ressource'!A1" display="'03_Ressource'!A1" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B11" location="'04_Infralineaire'!A1" display="'04_Infralineaire'!A1" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B12" location="'04_Environnement'!A1" display="'04_Environnement'!A1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B13" location="'04_Equipement'!A1" display="'04_Equipement'!A1" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B14" location="'04_Etudestrategie'!A1" display="'04_Etudestrategie'!A1" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B15" location="'04_Noeud'!A1" display="'04_Noeud'!A1" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B16" location="'04_Observation'!A1" display="'04_Observation'!A1" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B17" location="'04_Profil'!A1" display="'04_Profil'!A1" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B18" location="'05_Graphique'!A1" display="'05_Graphique'!A1" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B19" location="'05_Modele'!A1" display="'05_Modele'!A1" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B20" location="'05_Photo'!A1" display="'05_Photo'!A1" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B21" location="'05_Rapport'!A1" display="'05_Rapport'!A1" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B22" location="'05_Rasters'!A1" display="'05_Rasters'!A1" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B23" location="'05_Topographie'!A1" display="'05_Topographie'!A1" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B24" location="'05_Travaux'!A1" display="'05_Travaux'!A1" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B25" location="'06_Graphiquedata'!A1" display="'06_Graphiquedata'!A1" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B26" location="'06_Pointtopo'!A1" display="'06_Pointtopo'!A1" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B27" location="'06_Tcetudetravaux'!A1" display="'06_Tcetudetravaux'!A1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B28" location="'06_Tcobjetintervenant'!A1" display="'06_Tcobjetintervenant'!A1" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B29" location="'06_Tcobjetressource'!A1" display="'06_Tcobjetressource'!A1" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B30" location="'06_Tcobjetzonegeo'!A1" display="'06_Tcobjetzonegeo'!A1" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B31" location="'06_Tctravauxdescriptionsystem'!A1" display="'06_Tctravauxdescriptionsystem'!A1" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B32" location="'10_auth_group'!A1" display="'10_auth_group'!A1" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B33" location="'10_auth_group_permissions'!A1" display="'10_auth_group_permissions'!A1" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B34" location="'10_auth_permission'!A1" display="'10_auth_permission'!A1" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B35" location="'10_auth_user'!A1" display="'10_auth_user'!A1" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="B36" location="'10_auth_user_groups'!A1" display="'10_auth_user_groups'!A1" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B37" location="'10_auth_user_user_permissions'!A1" display="'10_auth_user_user_permissions'!A1" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B38" location="'10_bdd'!A1" display="'10_bdd'!A1" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B39" location="'10_carto_layer'!A1" display="'10_carto_layer'!A1" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B40" location="'10_django_admin_log'!A1" display="'10_django_admin_log'!A1" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B41" location="'10_django_content_type'!A1" display="'10_django_content_type'!A1" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B42" location="'10_django_migrations'!A1" display="'10_django_migrations'!A1" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B43" location="'10_django_session'!A1" display="'10_django_session'!A1" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B44" location="'10_messagetiers'!A1" display="'10_messagetiers'!A1" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B45" location="'10_projet'!A1" display="'10_projet'!A1" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B46" location="'10_siartelia'!A1" display="'10_siartelia'!A1" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B47" location="'11_utilisateur'!A1" display="'11_utilisateur'!A1" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B1" location="'00_Basedonnees'!A1" display="'00_Basedonnees'!A1"/>
+    <hyperlink ref="B2" location="'00_Revision'!A1" display="'00_Revision'!A1"/>
+    <hyperlink ref="B3" location="'01_Objet'!A1" display="'01_Objet'!A1"/>
+    <hyperlink ref="B4" location="'02_Descriptionsystem'!A1" display="'02_Descriptionsystem'!A1"/>
+    <hyperlink ref="B5" location="'02_Evenement'!A1" display="'02_Evenement'!A1"/>
+    <hyperlink ref="B6" location="'02_Marche'!A1" display="'02_Marche'!A1"/>
+    <hyperlink ref="B7" location="'02_Zonegeo'!A1" display="'02_Zonegeo'!A1"/>
+    <hyperlink ref="B8" location="'03_Desordre'!A1" display="'03_Desordre'!A1"/>
+    <hyperlink ref="B9" location="'03_Interventiontiers'!A1" display="'03_Interventiontiers'!A1"/>
+    <hyperlink ref="B10" location="'03_Ressource'!A1" display="'03_Ressource'!A1"/>
+    <hyperlink ref="B11" location="'04_Infralineaire'!A1" display="'04_Infralineaire'!A1"/>
+    <hyperlink ref="B12" location="'04_Environnement'!A1" display="'04_Environnement'!A1"/>
+    <hyperlink ref="B13" location="'04_Equipement'!A1" display="'04_Equipement'!A1"/>
+    <hyperlink ref="B14" location="'04_Etudestrategie'!A1" display="'04_Etudestrategie'!A1"/>
+    <hyperlink ref="B15" location="'04_Noeud'!A1" display="'04_Noeud'!A1"/>
+    <hyperlink ref="B16" location="'04_Observation'!A1" display="'04_Observation'!A1"/>
+    <hyperlink ref="B17" location="'04_Profil'!A1" display="'04_Profil'!A1"/>
+    <hyperlink ref="B18" location="'05_Graphique'!A1" display="'05_Graphique'!A1"/>
+    <hyperlink ref="B19" location="'05_Modele'!A1" display="'05_Modele'!A1"/>
+    <hyperlink ref="B20" location="'05_Photo'!A1" display="'05_Photo'!A1"/>
+    <hyperlink ref="B21" location="'05_Rapport'!A1" display="'05_Rapport'!A1"/>
+    <hyperlink ref="B22" location="'05_Rasters'!A1" display="'05_Rasters'!A1"/>
+    <hyperlink ref="B23" location="'05_Topographie'!A1" display="'05_Topographie'!A1"/>
+    <hyperlink ref="B24" location="'05_Travaux'!A1" display="'05_Travaux'!A1"/>
+    <hyperlink ref="B26" location="'06_Graphiquedata'!A1" display="'06_Graphiquedata'!A1"/>
+    <hyperlink ref="B27" location="'06_Pointtopo'!A1" display="'06_Pointtopo'!A1"/>
+    <hyperlink ref="B28" location="'06_Tcetudetravaux'!A1" display="'06_Tcetudetravaux'!A1"/>
+    <hyperlink ref="B29" location="'06_Tcobjetintervenant'!A1" display="'06_Tcobjetintervenant'!A1"/>
+    <hyperlink ref="B30" location="'06_Tcobjetressource'!A1" display="'06_Tcobjetressource'!A1"/>
+    <hyperlink ref="B31" location="'06_Tcobjetzonegeo'!A1" display="'06_Tcobjetzonegeo'!A1"/>
+    <hyperlink ref="B32" location="'06_Tctravauxdescriptionsystem'!A1" display="'06_Tctravauxdescriptionsystem'!A1"/>
+    <hyperlink ref="B33" location="'10_auth_group'!A1" display="'10_auth_group'!A1"/>
+    <hyperlink ref="B34" location="'10_auth_group_permissions'!A1" display="'10_auth_group_permissions'!A1"/>
+    <hyperlink ref="B35" location="'10_auth_permission'!A1" display="'10_auth_permission'!A1"/>
+    <hyperlink ref="B36" location="'10_auth_user'!A1" display="'10_auth_user'!A1"/>
+    <hyperlink ref="B37" location="'10_auth_user_groups'!A1" display="'10_auth_user_groups'!A1"/>
+    <hyperlink ref="B38" location="'10_auth_user_user_permissions'!A1" display="'10_auth_user_user_permissions'!A1"/>
+    <hyperlink ref="B39" location="'10_bdd'!A1" display="'10_bdd'!A1"/>
+    <hyperlink ref="B40" location="'10_carto_layer'!A1" display="'10_carto_layer'!A1"/>
+    <hyperlink ref="B41" location="'10_django_admin_log'!A1" display="'10_django_admin_log'!A1"/>
+    <hyperlink ref="B42" location="'10_django_content_type'!A1" display="'10_django_content_type'!A1"/>
+    <hyperlink ref="B43" location="'10_django_migrations'!A1" display="'10_django_migrations'!A1"/>
+    <hyperlink ref="B44" location="'10_django_session'!A1" display="'10_django_session'!A1"/>
+    <hyperlink ref="B45" location="'10_messagetiers'!A1" display="'10_messagetiers'!A1"/>
+    <hyperlink ref="B46" location="'10_projet'!A1" display="'10_projet'!A1"/>
+    <hyperlink ref="B47" location="'10_siartelia'!A1" display="'10_siartelia'!A1"/>
+    <hyperlink ref="B48" location="'11_utilisateur'!A1" display="'11_utilisateur'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2989,7 +2936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3220,7 +3167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3440,7 +3387,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3612,7 +3559,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3753,7 +3700,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3934,7 +3881,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4090,7 +4037,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4239,12 +4186,10 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4524,7 +4469,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4705,7 +4650,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4861,7 +4806,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4997,7 +4942,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5146,11 +5091,11 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
-  <dimension ref="A1:H14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5165,7 +5110,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>321</v>
+        <v>582</v>
       </c>
     </row>
     <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
@@ -5173,7 +5118,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>322</v>
+        <v>583</v>
       </c>
     </row>
     <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
@@ -5196,9 +5141,6 @@
       <c r="A5" t="s">
         <v>567</v>
       </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="6" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -5217,18 +5159,18 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>585</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>586</v>
       </c>
       <c r="H6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>323</v>
+      <c r="A7" s="19" t="s">
+        <v>579</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -5238,8 +5180,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>324</v>
+      <c r="A8" s="18" t="s">
+        <v>580</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
@@ -5249,7 +5191,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="19" t="s">
         <v>301</v>
       </c>
       <c r="B9" t="s">
@@ -5263,41 +5205,27 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>325</v>
+      <c r="A11" s="18" t="s">
+        <v>581</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>327</v>
-      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F12" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>294</v>
+      <c r="A12" t="s">
+        <v>585</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F13" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>224</v>
+      <c r="A13" t="s">
+        <v>586</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -5306,12 +5234,168 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.7109375" style="6" customWidth="1"/>
+    <col min="2" max="8" width="23.28515625" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>567</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A11:B11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5435,8 +5519,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5634,8 +5718,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5758,13 +5842,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5989,13 +6071,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6195,8 +6275,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6449,144 +6529,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
-  <dimension ref="A1:H15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.7109375" style="6" customWidth="1"/>
-    <col min="2" max="9" width="29.140625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>567</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>419</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>420</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>421</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6702,7 +6646,143 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" style="6" customWidth="1"/>
+    <col min="2" max="9" width="29.140625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>567</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>419</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>420</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>421</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6894,12 +6974,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A12" sqref="A11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7027,8 +7107,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7162,8 +7242,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7296,8 +7376,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7358,8 +7438,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7428,8 +7508,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7506,8 +7586,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7702,8 +7782,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7772,78 +7852,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26" style="10" customWidth="1"/>
-    <col min="2" max="10" width="19" style="10" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>458</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>466</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -8059,7 +8069,77 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" style="10" customWidth="1"/>
+    <col min="2" max="10" width="19" style="10" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8152,8 +8232,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8254,8 +8334,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8364,8 +8444,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8434,8 +8514,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8512,8 +8592,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8582,8 +8662,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8728,8 +8808,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8870,8 +8950,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8924,85 +9004,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
-  <dimension ref="A1:H4"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.28515625" style="10" customWidth="1"/>
-    <col min="2" max="8" width="24.7109375" style="10" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>563</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>458</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>564</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>565</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J74"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9412,174 +9419,87 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="11" t="s">
-        <v>579</v>
-      </c>
-      <c r="B55" s="18" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
-        <v>580</v>
-      </c>
-      <c r="B56" s="18" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
-        <v>581</v>
-      </c>
-      <c r="B57" s="18" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
-        <v>582</v>
-      </c>
-      <c r="B58" s="18" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
-        <v>583</v>
-      </c>
-      <c r="B59" s="18" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
-        <v>584</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
-        <v>585</v>
-      </c>
-      <c r="B61" s="18" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
-        <v>586</v>
-      </c>
-      <c r="B62" s="18" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
-        <v>587</v>
-      </c>
-      <c r="B63" s="18" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
-        <v>588</v>
-      </c>
-      <c r="B64" s="18" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
-        <v>589</v>
-      </c>
-      <c r="B65" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
-        <v>590</v>
-      </c>
-      <c r="B66" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
-        <v>591</v>
-      </c>
-      <c r="B67" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
-        <v>592</v>
-      </c>
-      <c r="B68" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
-        <v>593</v>
-      </c>
-      <c r="B69" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
-        <v>594</v>
-      </c>
-      <c r="B70" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
-        <v>595</v>
-      </c>
-      <c r="B71" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
-        <v>596</v>
-      </c>
-      <c r="B72" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
-        <v>597</v>
-      </c>
-      <c r="B73" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>598</v>
-      </c>
-      <c r="B74" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" style="10" customWidth="1"/>
+    <col min="2" max="8" width="24.7109375" style="10" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>563</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>564</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>565</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -9751,11 +9671,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9934,7 +9854,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -10077,7 +9997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>